<commit_message>
added postal levels (#2)
</commit_message>
<xml_diff>
--- a/11.1.3/IBM CA 11.1 Administrative Hierarchy.xlsx
+++ b/11.1.3/IBM CA 11.1 Administrative Hierarchy.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GJF\Endor\Atlas\CustomerDocumentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC02620-A549-46A0-BC30-4DE301E883C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D93CDCD-D6CA-45A3-8DA4-4D12D700AE2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="405" windowWidth="25815" windowHeight="13530" xr2:uid="{1E9FF073-40CC-4252-9A71-28BF98A0B578}"/>
+    <workbookView xWindow="31335" yWindow="2925" windowWidth="21600" windowHeight="11325" xr2:uid="{1E9FF073-40CC-4252-9A71-28BF98A0B578}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="951">
   <si>
     <t>Country Code</t>
   </si>
@@ -2989,57 +2984,6 @@
     <cellStyle name="Standard_Tabelle1" xfId="1" xr:uid="{25B49457-DBC8-490E-BC36-66F77682AB78}"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3210,6 +3154,57 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3224,16 +3219,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03049C57-9F28-4415-B43F-885BEEE7C04A}" name="Table1" displayName="Table1" ref="A1:G249" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="Normal_GiStatus_51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03049C57-9F28-4415-B43F-885BEEE7C04A}" name="Table1" displayName="Table1" ref="A1:G249" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Normal_GiStatus_51">
   <autoFilter ref="A1:G249" xr:uid="{E70307FA-354C-4DD3-94DF-0D9B101608D7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{09EBD41E-2536-4A67-804A-97A36AE19028}" name="Country Code" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{51D34EF3-7C20-4BC9-978C-E026990D9DD1}" name="Country Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F4C79FED-4DB2-46F1-BFA7-66F5CA3AEA93}" name="Administrative Level 1" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2B612616-224A-45C4-B62B-4D213C521DAA}" name="Administrative Level 2" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4AC9FC96-1454-43AD-B9E4-03026E4DC772}" name="Administrative Level 3" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{8EB9996B-D9C8-4B27-A32D-50D56969A202}" name="Administrative Level 4" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{278B8839-5B9B-49E2-BBAA-7D863351FEFD}" name="Administrative Level 5" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{09EBD41E-2536-4A67-804A-97A36AE19028}" name="Country Code" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{51D34EF3-7C20-4BC9-978C-E026990D9DD1}" name="Country Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F4C79FED-4DB2-46F1-BFA7-66F5CA3AEA93}" name="Administrative Level 1" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2B612616-224A-45C4-B62B-4D213C521DAA}" name="Administrative Level 2" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4AC9FC96-1454-43AD-B9E4-03026E4DC772}" name="Administrative Level 3" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8EB9996B-D9C8-4B27-A32D-50D56969A202}" name="Administrative Level 4" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{278B8839-5B9B-49E2-BBAA-7D863351FEFD}" name="Administrative Level 5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>